<commit_message>
conceptos terminados sin sverificar
</commit_message>
<xml_diff>
--- a/public/storage/pruebas/files_up/conceptos5.xlsx
+++ b/public/storage/pruebas/files_up/conceptos5.xlsx
@@ -586,7 +586,7 @@
         <v>21</v>
       </c>
       <c r="H2">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -627,7 +627,7 @@
         <v>21</v>
       </c>
       <c r="H3">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -665,7 +665,7 @@
         <v>21</v>
       </c>
       <c r="H4">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -706,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="H5">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>21</v>
       </c>
       <c r="H6">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -782,7 +782,7 @@
         <v>21</v>
       </c>
       <c r="H7">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -820,7 +820,7 @@
         <v>21</v>
       </c>
       <c r="H8">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -861,7 +861,7 @@
         <v>21</v>
       </c>
       <c r="H9">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -899,7 +899,7 @@
         <v>21</v>
       </c>
       <c r="H10">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -928,7 +928,7 @@
         <v>21</v>
       </c>
       <c r="H11">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -969,7 +969,7 @@
         <v>21</v>
       </c>
       <c r="H12">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1010,7 +1010,7 @@
         <v>21</v>
       </c>
       <c r="H13">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1051,7 +1051,7 @@
         <v>21</v>
       </c>
       <c r="H14">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1092,7 +1092,7 @@
         <v>21</v>
       </c>
       <c r="H15">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1133,7 +1133,7 @@
         <v>21</v>
       </c>
       <c r="H16">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1174,7 +1174,7 @@
         <v>21</v>
       </c>
       <c r="H17">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1215,7 +1215,7 @@
         <v>21</v>
       </c>
       <c r="H18">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -1256,7 +1256,7 @@
         <v>21</v>
       </c>
       <c r="H19">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1285,7 +1285,7 @@
         <v>21</v>
       </c>
       <c r="H20">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="I20">
         <v>1</v>

</xml_diff>